<commit_message>
Back to wells G
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertwang/Desktop/cytometry-tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65E26D1-18A6-EC43-94CA-D2019BAE2848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B73370-0261-6B4C-9A8F-2D9DBA5C24A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15540" xr2:uid="{33BFC1F3-22F5-A94A-95E8-D8059F13A24B}"/>
   </bookViews>
@@ -43,40 +43,40 @@
     <t>IPTG</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
-    <t>F5</t>
-  </si>
-  <si>
-    <t>F6</t>
-  </si>
-  <si>
-    <t>F7</t>
-  </si>
-  <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>F9</t>
-  </si>
-  <si>
-    <t>F10</t>
-  </si>
-  <si>
-    <t>F11</t>
-  </si>
-  <si>
-    <t>F12</t>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G12</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>